<commit_message>
Update outputs of reliability module to show subsytems consumed by the maintenance module.
Modify for changes in dtocean-reliability API
</commit_message>
<xml_diff>
--- a/dds/reliability.xlsx
+++ b/dds/reliability.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8080" tabRatio="356" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8080" tabRatio="437"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="181">
   <si>
     <t>Identifier</t>
   </si>
@@ -125,12 +125,6 @@
     <t>Unit 3</t>
   </si>
   <si>
-    <t>Unit …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Failures per 10^{6} hours </t>
-  </si>
-  <si>
     <t>Table 1</t>
   </si>
   <si>
@@ -395,21 +389,9 @@
     <t>SimpleData</t>
   </si>
   <si>
-    <t>Mean Time to Failure of the System</t>
-  </si>
-  <si>
     <t>NumpyLine</t>
   </si>
   <si>
-    <t>System Reliability at Mission Time</t>
-  </si>
-  <si>
-    <t>System reliability</t>
-  </si>
-  <si>
-    <t>Time [hours]</t>
-  </si>
-  <si>
     <t>Required system Mean Time to Failure (% of the Mission Time)</t>
   </si>
   <si>
@@ -452,45 +434,9 @@
     <t>Required System Mean Time to Failure (% of the Mission Time)</t>
   </si>
   <si>
-    <t>System Reliability at Array Level</t>
-  </si>
-  <si>
-    <t>SimpleDict</t>
-  </si>
-  <si>
-    <t>Subsystem Reliability - Substation</t>
-  </si>
-  <si>
-    <t>Subsystem Mean Time to Failure  - Substation</t>
-  </si>
-  <si>
-    <t>Subsystem Reliability - Export cable</t>
-  </si>
-  <si>
-    <t>Subsystem Mean Time to Failure  - Export cable</t>
-  </si>
-  <si>
-    <t>Subsystem Mean Time to Failure  - Export Cable</t>
-  </si>
-  <si>
-    <t>Subsystem Reliability - Electrical Subsystem per Device</t>
-  </si>
-  <si>
-    <t>Subsystem Mean Time to Failure  - Electrical Subsystem per Device</t>
-  </si>
-  <si>
-    <t>Subsystem Reliability - Moorings and Foundations Subsystem per Device</t>
-  </si>
-  <si>
-    <t>Subsystem Mean Time to Failure  - Moorings and Foundations Subsystem per Device</t>
-  </si>
-  <si>
     <t>hours</t>
   </si>
   <si>
-    <t>1 / hours</t>
-  </si>
-  <si>
     <t>reference.view_component_collection_point</t>
   </si>
   <si>
@@ -539,44 +485,131 @@
     <t>project.rsystime</t>
   </si>
   <si>
-    <t>project.rarrayvalue2</t>
-  </si>
-  <si>
     <t>project.export_cable_reliability</t>
   </si>
   <si>
-    <t>project.export_cable_mttf</t>
-  </si>
-  <si>
     <t>project.substation_reliability</t>
   </si>
   <si>
-    <t>project.substation_mttf</t>
-  </si>
-  <si>
-    <t>project.elec_subsystem_reliability</t>
-  </si>
-  <si>
-    <t>project.elec_subsystem_mttf</t>
-  </si>
-  <si>
-    <t>project.moor_found_reliability</t>
-  </si>
-  <si>
-    <t>project.moor_found_mttf</t>
+    <t>Failures per 10^{6} hours</t>
+  </si>
+  <si>
+    <t>Unit 4</t>
+  </si>
+  <si>
+    <t>Failure Rate</t>
+  </si>
+  <si>
+    <t>MTTF</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>project.moorings_reliability</t>
+  </si>
+  <si>
+    <t>project.interarray_cable_reliability</t>
+  </si>
+  <si>
+    <t>project.umbilical_cable_reliability</t>
+  </si>
+  <si>
+    <t>project.hub_reliability</t>
+  </si>
+  <si>
+    <t>TableData</t>
+  </si>
+  <si>
+    <t>Failure rate and mean time to failure for each collection hub</t>
+  </si>
+  <si>
+    <t>System ID</t>
+  </si>
+  <si>
+    <t>Array Reliability at Mission Time</t>
+  </si>
+  <si>
+    <t>Mean Time to Failure of the Array</t>
+  </si>
+  <si>
+    <t>The evolution of the reliability of the array during the mission time</t>
+  </si>
+  <si>
+    <t>Failure rate and mean time to failure for the array export cable and connectors</t>
+  </si>
+  <si>
+    <t>Failure rate and mean time to failure for the inter-array cables and connectors of each device or collection hub</t>
+  </si>
+  <si>
+    <t>Failure rate and mean time to failure for the array substation systems</t>
+  </si>
+  <si>
+    <t>Export Cable Sub-System Reliability Metrics</t>
+  </si>
+  <si>
+    <t>Substation Sub-System Reliability Metrics</t>
+  </si>
+  <si>
+    <t>Collection Hub Sub-System Reliability Metrics</t>
+  </si>
+  <si>
+    <t>Inter-Array Cable Sub-System Reliability Metrics</t>
+  </si>
+  <si>
+    <t>Umbilical Cable Sub-System Reliability Metrics</t>
+  </si>
+  <si>
+    <t>Moorings and Foundations Sub-System Reliability Metrics</t>
+  </si>
+  <si>
+    <t>Failure rate and mean time to failure for the moorings and foundation systems of each device</t>
+  </si>
+  <si>
+    <t>Failure rate and mean time to failure for the umbilical cables and connectors of each device</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>System Reliability</t>
+  </si>
+  <si>
+    <t>Mean time to failure (MTTF) for the first component in the array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -613,7 +646,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,12 +657,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFCD5B5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -682,33 +709,35 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -1089,10 +1118,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AMK39"/>
+  <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1101,7 +1130,7 @@
     <col min="2" max="2" width="16.36328125" style="1"/>
     <col min="3" max="3" width="19" style="1"/>
     <col min="4" max="4" width="73.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="53.54296875" style="1" customWidth="1"/>
     <col min="6" max="12" width="9" style="1"/>
     <col min="13" max="13" width="23.08984375" style="1"/>
     <col min="14" max="1025" width="19.90625" style="1"/>
@@ -1148,536 +1177,498 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="B4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="B5" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="11" t="s">
+    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="B8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="B9" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="B10" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="B11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+    <row r="12" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="B12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="B13" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="B16" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="B17" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="B18" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="B19" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="B20" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="B21" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="11" t="s">
+      <c r="B22" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="E22" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="B23" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E23" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="11" t="s">
+    <row r="25" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="11" t="s">
+    <row r="26" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="11" t="s">
+      <c r="D28" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
+      <c r="D30" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
+    </row>
+    <row r="31" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E31" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
+    </row>
+    <row r="32" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13" t="s">
-        <v>172</v>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
-        <v>173</v>
+        <v>161</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
+      <c r="E36" s="14" t="s">
         <v>176</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1692,10 +1683,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1740,455 +1731,533 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" t="s">
+        <v>154</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2205,10 +2274,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:Z39"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2257,7 +2326,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -2274,7 +2343,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -2291,7 +2360,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -2308,7 +2377,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -2325,7 +2394,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -2342,7 +2411,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -2359,7 +2428,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -2376,7 +2445,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -2393,7 +2462,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -2410,7 +2479,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -2427,7 +2496,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -2444,7 +2513,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -2461,7 +2530,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -2478,7 +2547,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -2495,7 +2564,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -2512,7 +2581,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -2529,7 +2598,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
@@ -2546,7 +2615,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -2563,7 +2632,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -2580,7 +2649,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -2597,7 +2666,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
@@ -2614,7 +2683,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -2631,7 +2700,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -2648,7 +2717,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -2665,7 +2734,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -2682,7 +2751,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -2699,7 +2768,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -2707,7 +2776,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -2718,81 +2787,87 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
-        <v>169</v>
+      <c r="A31" t="s">
+        <v>150</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
       </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
-        <v>170</v>
+      <c r="A32" t="s">
+        <v>151</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
-        <v>171</v>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
-        <v>172</v>
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="8" t="s">
-        <v>173</v>
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
-        <v>174</v>
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>157</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2807,16 +2882,18 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.08984375"/>
-    <col min="2" max="1025" width="19.90625"/>
+    <col min="1" max="1" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+    <col min="3" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="1025" width="19.90625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -2833,548 +2910,554 @@
         <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="B31" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="B34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B39" t="s">
-        <v>150</v>
-      </c>
-      <c r="C39" t="s">
-        <v>151</v>
+      <c r="B32" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3390,7 +3473,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3407,542 +3490,542 @@
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F8" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F12" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F13" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F22" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F24" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F25" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F26" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="F27" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -3967,7 +4050,7 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L33" sqref="A2:L33"/>
     </sheetView>
   </sheetViews>
@@ -3982,16 +4065,16 @@
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add variable project.mttf_test to capture whether the design mean time to first failure was exceeded
</commit_message>
<xml_diff>
--- a/dds/reliability.xlsx
+++ b/dds/reliability.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="185">
   <si>
     <t>Identifier</t>
   </si>
@@ -392,9 +392,6 @@
     <t>NumpyLine</t>
   </si>
   <si>
-    <t>Required system Mean Time to Failure (% of the Mission Time)</t>
-  </si>
-  <si>
     <t>component_id</t>
   </si>
   <si>
@@ -431,9 +428,6 @@
     <t>Mooring Shackle Critical Failure Rates</t>
   </si>
   <si>
-    <t>Required System Mean Time to Failure (% of the Mission Time)</t>
-  </si>
-  <si>
     <t>hours</t>
   </si>
   <si>
@@ -530,9 +524,6 @@
     <t>Array Reliability at Mission Time</t>
   </si>
   <si>
-    <t>Mean Time to Failure of the Array</t>
-  </si>
-  <si>
     <t>The evolution of the reliability of the array during the mission time</t>
   </si>
   <si>
@@ -575,7 +566,28 @@
     <t>System Reliability</t>
   </si>
   <si>
-    <t>Mean time to failure (MTTF) for the first component in the array</t>
+    <t>Mean time to the first failure of a component within the array</t>
+  </si>
+  <si>
+    <t>project.mttf_test</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Mean Time to First Failure</t>
+  </si>
+  <si>
+    <t>Design Mean Time to First Failure</t>
+  </si>
+  <si>
+    <t>Design mean time to the first failure of a component within the array</t>
+  </si>
+  <si>
+    <t>Mean Time to First Failure Within Design Limits</t>
+  </si>
+  <si>
+    <t>Is the mean time to failure of the first component within the design limits?</t>
   </si>
 </sst>
 </file>
@@ -715,7 +727,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -737,6 +749,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
@@ -1118,10 +1131,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AMK36"/>
+  <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1182,7 +1195,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>43</v>
@@ -1196,7 +1209,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>45</v>
@@ -1210,7 +1223,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>49</v>
@@ -1224,7 +1237,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>51</v>
@@ -1238,7 +1251,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>53</v>
@@ -1252,7 +1265,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>47</v>
@@ -1266,7 +1279,7 @@
         <v>55</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>62</v>
@@ -1280,7 +1293,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>63</v>
@@ -1294,7 +1307,7 @@
         <v>57</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>64</v>
@@ -1308,7 +1321,7 @@
         <v>58</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>65</v>
@@ -1322,7 +1335,7 @@
         <v>59</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>66</v>
@@ -1336,7 +1349,7 @@
         <v>60</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>61</v>
@@ -1350,7 +1363,7 @@
         <v>76</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>90</v>
@@ -1364,7 +1377,7 @@
         <v>77</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>92</v>
@@ -1378,7 +1391,7 @@
         <v>78</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>94</v>
@@ -1392,7 +1405,7 @@
         <v>79</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>96</v>
@@ -1406,7 +1419,7 @@
         <v>80</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>98</v>
@@ -1420,7 +1433,7 @@
         <v>81</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>100</v>
@@ -1434,7 +1447,7 @@
         <v>82</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>102</v>
@@ -1448,7 +1461,7 @@
         <v>83</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>104</v>
@@ -1462,7 +1475,7 @@
         <v>84</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>105</v>
@@ -1476,7 +1489,7 @@
         <v>85</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>106</v>
@@ -1490,7 +1503,7 @@
         <v>86</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>107</v>
@@ -1504,7 +1517,7 @@
         <v>87</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>108</v>
@@ -1518,10 +1531,10 @@
         <v>88</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>114</v>
@@ -1532,7 +1545,7 @@
         <v>89</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>109</v>
@@ -1543,87 +1556,86 @@
     </row>
     <row r="28" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>119</v>
+      <c r="D28" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="E29" s="15" t="s">
+      <c r="D29" s="16" t="s">
         <v>180</v>
       </c>
+      <c r="E29" s="16" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="30" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>149</v>
+      <c r="A30" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>166</v>
+        <v>117</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>161</v>
+        <v>147</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="C33" s="12"/>
+        <v>159</v>
+      </c>
       <c r="D33" s="14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1631,29 +1643,29 @@
         <v>158</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>161</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1661,14 +1673,29 @@
         <v>157</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="14" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2173,91 +2200,91 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2274,10 +2301,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2768,7 +2795,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -2776,7 +2803,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -2787,7 +2814,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
@@ -2795,7 +2822,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -2806,7 +2833,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -2817,7 +2844,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
@@ -2831,7 +2858,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
@@ -2845,7 +2872,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
@@ -2859,7 +2886,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
@@ -2869,6 +2896,14 @@
       </c>
       <c r="D36" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2885,7 +2920,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2910,7 +2945,7 @@
         <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2921,13 +2956,13 @@
         <v>26</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -2938,13 +2973,13 @@
         <v>26</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2955,13 +2990,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -2972,13 +3007,13 @@
         <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2989,13 +3024,13 @@
         <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -3006,13 +3041,13 @@
         <v>26</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -3023,13 +3058,13 @@
         <v>26</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -3040,13 +3075,13 @@
         <v>26</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -3057,13 +3092,13 @@
         <v>26</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -3074,13 +3109,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -3091,13 +3126,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -3108,13 +3143,13 @@
         <v>26</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -3125,13 +3160,13 @@
         <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -3142,13 +3177,13 @@
         <v>26</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -3159,13 +3194,13 @@
         <v>26</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -3176,13 +3211,13 @@
         <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -3193,13 +3228,13 @@
         <v>26</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -3210,13 +3245,13 @@
         <v>26</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -3227,13 +3262,13 @@
         <v>26</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -3244,13 +3279,13 @@
         <v>26</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -3261,13 +3296,13 @@
         <v>26</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -3278,13 +3313,13 @@
         <v>26</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -3295,13 +3330,13 @@
         <v>26</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -3312,13 +3347,13 @@
         <v>26</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -3329,13 +3364,13 @@
         <v>26</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -3346,37 +3381,37 @@
         <v>26</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
         <v>26</v>
@@ -3384,80 +3419,80 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3499,13 +3534,13 @@
         <v>32</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -3513,19 +3548,19 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -3533,19 +3568,19 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -3553,19 +3588,19 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E4" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -3573,19 +3608,19 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -3593,19 +3628,19 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E6" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -3613,19 +3648,19 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -3633,19 +3668,19 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -3653,19 +3688,19 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -3673,19 +3708,19 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -3693,19 +3728,19 @@
         <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -3713,19 +3748,19 @@
         <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -3733,19 +3768,19 @@
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -3753,19 +3788,19 @@
         <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E14" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -3773,19 +3808,19 @@
         <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E15" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -3793,19 +3828,19 @@
         <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E16" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -3813,19 +3848,19 @@
         <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -3833,19 +3868,19 @@
         <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E18" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -3853,19 +3888,19 @@
         <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E19" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -3873,19 +3908,19 @@
         <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E20" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -3893,19 +3928,19 @@
         <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -3913,19 +3948,19 @@
         <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -3933,19 +3968,19 @@
         <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -3953,19 +3988,19 @@
         <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -3973,19 +4008,19 @@
         <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -3993,19 +4028,19 @@
         <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -4013,19 +4048,19 @@
         <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add static cable kfactors to reliability and maintenance interfaces
</commit_message>
<xml_diff>
--- a/dds/reliability.xlsx
+++ b/dds/reliability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F33A41D-5C67-4B8A-A205-0904FC66CBD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AD7B5A-CB3F-47D6-9D0D-FFD698380006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="229">
   <si>
     <t>Identifier</t>
   </si>
@@ -685,19 +685,62 @@
   </si>
   <si>
     <t>Non-critical reliability metrics for the device sub-systems (i.e. PTO, prime mover, support structure and control system)</t>
+  </si>
+  <si>
+    <t>project.apply_kfactors</t>
+  </si>
+  <si>
+    <t>Apply k-factors</t>
+  </si>
+  <si>
+    <t>component.static_cable_perkm_NCFR</t>
+  </si>
+  <si>
+    <t>Static Cable Non-Critical Per km Failure Rates</t>
+  </si>
+  <si>
+    <t>component.static_cable_perkm_CFR</t>
+  </si>
+  <si>
+    <t>Static Cable Critical Per km Failure Rates</t>
+  </si>
+  <si>
+    <t>Failures per 10^{6} hours per km</t>
+  </si>
+  <si>
+    <t>Non-critical per km failure rates for static cables. Used in k-factor calculation.</t>
+  </si>
+  <si>
+    <t>Critical per km failure rates for static cables. Used in k-factor calculation.</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Label_5</t>
+  </si>
+  <si>
+    <t>Use k-factors for failure rate adjustment. Default is False.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -735,14 +778,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFB9CDE5"/>
+        <fgColor rgb="FFB9CDE5"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB9CDE5"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -775,31 +818,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="60% - Accent3" xfId="2" builtinId="40"/>
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1184,10 +1230,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:AMK47"/>
+  <dimension ref="A1:AMK50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,607 +1347,649 @@
     </row>
     <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>219</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>220</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>47</v>
+        <v>221</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>48</v>
+        <v>222</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>49</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="30" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B30" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D30" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E30" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="31" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D31" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E31" s="11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+    <row r="32" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10" t="s">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="34" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10" t="s">
+      <c r="C34" s="9"/>
+      <c r="D34" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+    <row r="35" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10" t="s">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    <row r="36" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10" t="s">
+      <c r="C36" s="9"/>
+      <c r="D36" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="37" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="38" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10" t="s">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="39" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10" t="s">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+    <row r="40" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10" t="s">
+      <c r="C40" s="9"/>
+      <c r="D40" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E40" s="9" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+    <row r="41" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10" t="s">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+    <row r="42" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="43" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10" t="s">
+      <c r="C43" s="9"/>
+      <c r="D43" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+    <row r="44" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E44" s="9" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+    <row r="45" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10" t="s">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+    <row r="46" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10" t="s">
+      <c r="C46" s="9"/>
+      <c r="D46" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E46" s="9" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+    <row r="47" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10" t="s">
+      <c r="C47" s="9"/>
+      <c r="D47" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E47" s="9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+    <row r="48" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10" t="s">
+      <c r="C48" s="9"/>
+      <c r="D48" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E48" s="9" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+    <row r="49" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10" t="s">
+      <c r="C49" s="9"/>
+      <c r="D49" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E49" s="9" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+    <row r="50" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10" t="s">
+      <c r="C50" s="9"/>
+      <c r="D50" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E50" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -1917,10 +2005,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,7 +2018,7 @@
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
     <col min="9" max="10" width="23.5703125" customWidth="1"/>
@@ -1946,25 +2034,28 @@
     <col min="28" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="F1" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -1980,7 +2071,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1997,7 +2088,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2014,7 +2105,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2031,9 +2122,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
         <v>99</v>
@@ -2048,9 +2139,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>99</v>
@@ -2065,9 +2156,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>32</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
@@ -2082,9 +2173,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -2099,9 +2190,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
@@ -2116,9 +2207,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -2133,9 +2224,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -2150,9 +2241,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>221</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
@@ -2167,9 +2258,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>99</v>
@@ -2184,9 +2275,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>53</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
@@ -2201,9 +2292,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>99</v>
@@ -2220,7 +2311,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>99</v>
@@ -2237,7 +2328,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>99</v>
@@ -2254,7 +2345,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>99</v>
@@ -2271,7 +2362,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>99</v>
@@ -2288,7 +2379,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>99</v>
@@ -2305,7 +2396,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>99</v>
@@ -2322,7 +2413,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>99</v>
@@ -2339,7 +2430,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>99</v>
@@ -2356,7 +2447,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>99</v>
@@ -2373,7 +2464,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
         <v>99</v>
@@ -2390,7 +2481,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
         <v>99</v>
@@ -2406,48 +2497,42 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>159</v>
+      <c r="A28" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
-        <v>158</v>
-      </c>
-      <c r="F28" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>194</v>
+      <c r="A29" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>158</v>
-      </c>
-      <c r="F29" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="B30" t="s">
         <v>105</v>
@@ -2467,7 +2552,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="B31" t="s">
         <v>105</v>
@@ -2487,7 +2572,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -2507,7 +2592,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s">
         <v>105</v>
@@ -2527,7 +2612,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
         <v>105</v>
@@ -2547,7 +2632,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
         <v>105</v>
@@ -2567,7 +2652,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>211</v>
+        <v>171</v>
       </c>
       <c r="B36" t="s">
         <v>105</v>
@@ -2587,7 +2672,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B37" t="s">
         <v>105</v>
@@ -2607,7 +2692,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
         <v>105</v>
@@ -2627,7 +2712,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B39" t="s">
         <v>105</v>
@@ -2647,7 +2732,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B40" t="s">
         <v>105</v>
@@ -2667,7 +2752,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B41" t="s">
         <v>105</v>
@@ -2687,7 +2772,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="B42" t="s">
         <v>105</v>
@@ -2707,7 +2792,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B43" t="s">
         <v>105</v>
@@ -2727,7 +2812,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B44" t="s">
         <v>105</v>
@@ -2747,7 +2832,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B45" t="s">
         <v>105</v>
@@ -2762,6 +2847,46 @@
         <v>158</v>
       </c>
       <c r="F45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" t="s">
+        <v>158</v>
+      </c>
+      <c r="F47" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2776,10 +2901,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,45 +2914,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -2896,7 +3021,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
         <v>111</v>
@@ -2913,7 +3038,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>111</v>
@@ -2929,8 +3054,8 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>32</v>
+      <c r="A8" t="s">
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>111</v>
@@ -2946,8 +3071,8 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
+      <c r="A9" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>111</v>
@@ -2964,7 +3089,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>111</v>
@@ -2981,7 +3106,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>111</v>
@@ -2998,7 +3123,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>111</v>
@@ -3015,7 +3140,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>221</v>
       </c>
       <c r="B13" t="s">
         <v>111</v>
@@ -3031,8 +3156,8 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
+      <c r="A14" t="s">
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>111</v>
@@ -3048,8 +3173,8 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>53</v>
+      <c r="A15" t="s">
+        <v>47</v>
       </c>
       <c r="B15" t="s">
         <v>111</v>
@@ -3066,7 +3191,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>111</v>
@@ -3081,9 +3206,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>111</v>
@@ -3098,9 +3223,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>111</v>
@@ -3115,9 +3240,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>111</v>
@@ -3132,9 +3257,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>111</v>
@@ -3149,9 +3274,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>111</v>
@@ -3166,9 +3291,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>111</v>
@@ -3183,9 +3308,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>111</v>
@@ -3200,9 +3325,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>111</v>
@@ -3217,9 +3342,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
@@ -3234,9 +3359,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
         <v>111</v>
@@ -3251,9 +3376,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
         <v>111</v>
@@ -3268,85 +3393,67 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>151</v>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>152</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" t="s">
         <v>155</v>
       </c>
-      <c r="F30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>194</v>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B31" t="s">
         <v>111</v>
       </c>
-      <c r="C31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" t="s">
-        <v>155</v>
-      </c>
-      <c r="F31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" t="s">
-        <v>155</v>
-      </c>
-      <c r="F32" t="s">
-        <v>112</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B33" t="s">
         <v>111</v>
@@ -3366,7 +3473,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
         <v>111</v>
@@ -3386,7 +3493,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>197</v>
       </c>
       <c r="B35" t="s">
         <v>111</v>
@@ -3406,7 +3513,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B36" t="s">
         <v>111</v>
@@ -3426,7 +3533,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
         <v>111</v>
@@ -3446,7 +3553,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
         <v>111</v>
@@ -3466,7 +3573,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B39" t="s">
         <v>111</v>
@@ -3486,7 +3593,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
         <v>111</v>
@@ -3506,7 +3613,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B41" t="s">
         <v>111</v>
@@ -3526,7 +3633,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="B42" t="s">
         <v>111</v>
@@ -3546,7 +3653,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="B43" t="s">
         <v>111</v>
@@ -3566,7 +3673,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="B44" t="s">
         <v>111</v>
@@ -3586,7 +3693,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="B45" t="s">
         <v>111</v>
@@ -3606,7 +3713,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B46" t="s">
         <v>111</v>
@@ -3626,7 +3733,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="B47" t="s">
         <v>111</v>
@@ -3641,6 +3748,66 @@
         <v>155</v>
       </c>
       <c r="F47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>182</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" t="s">
+        <v>155</v>
+      </c>
+      <c r="F48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>183</v>
+      </c>
+      <c r="B49" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" t="s">
+        <v>155</v>
+      </c>
+      <c r="F49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" t="s">
+        <v>112</v>
+      </c>
+      <c r="E50" t="s">
+        <v>155</v>
+      </c>
+      <c r="F50" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3655,40 +3822,41 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="5" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="6" max="1025" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -3757,58 +3925,58 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
         <v>117</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>117</v>
@@ -3825,7 +3993,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>117</v>
@@ -3842,7 +4010,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>117</v>
@@ -3859,7 +4027,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>117</v>
@@ -3876,41 +4044,41 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="B15" t="s">
         <v>117</v>
@@ -3927,7 +4095,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>117</v>
@@ -3944,7 +4112,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>117</v>
@@ -3961,7 +4129,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>117</v>
@@ -3978,7 +4146,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>117</v>
@@ -3995,7 +4163,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>117</v>
@@ -4012,7 +4180,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>117</v>
@@ -4029,7 +4197,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>117</v>
@@ -4046,7 +4214,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>117</v>
@@ -4063,7 +4231,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>117</v>
@@ -4080,7 +4248,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>117</v>
@@ -4097,7 +4265,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
         <v>117</v>
@@ -4114,72 +4282,66 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B27" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>117</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D29" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" t="s">
-        <v>117</v>
+      <c r="D29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" t="s">
-        <v>117</v>
+        <v>151</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>117</v>
@@ -4199,7 +4361,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>117</v>
@@ -4219,7 +4381,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>117</v>
@@ -4239,7 +4401,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>117</v>
@@ -4259,7 +4421,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>117</v>
@@ -4279,7 +4441,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>117</v>
@@ -4299,7 +4461,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>171</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>117</v>
@@ -4319,7 +4481,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>117</v>
@@ -4339,7 +4501,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>117</v>
@@ -4359,7 +4521,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>117</v>
@@ -4379,7 +4541,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>117</v>
@@ -4399,7 +4561,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>117</v>
@@ -4419,7 +4581,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>117</v>
@@ -4439,7 +4601,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>117</v>
@@ -4459,7 +4621,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>117</v>
@@ -4479,7 +4641,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>117</v>
@@ -4494,6 +4656,46 @@
         <v>117</v>
       </c>
       <c r="F46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4510,7 +4712,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4522,31 +4724,31 @@
     <col min="4" max="1025" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -4666,7 +4868,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
@@ -5088,20 +5290,20 @@
     <col min="2" max="1025" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>